<commit_message>
Creates animation and saves mp4. Still need subplot of chArea line and average.
</commit_message>
<xml_diff>
--- a/DummyData.xlsx
+++ b/DummyData.xlsx
@@ -371,7 +371,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -395,10 +395,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>92.391420174562072</v>
@@ -412,10 +412,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>221.01858710297367</v>
@@ -429,10 +429,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>254.37048876046327</v>
@@ -446,10 +446,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>37.710153952994538</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>71.445981476421579</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>106.47960121162127</v>
@@ -463,10 +463,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>92.421329895245648</v>
+        <v>100</v>
       </c>
       <c r="B6">
-        <v>3.2959296670790894</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>176.10353635652913</v>

</xml_diff>